<commit_message>
OPC item values now read line by line, still only handles string values though
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>item2</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>value9</t>
+  </si>
+  <si>
+    <t>item1</t>
+  </si>
+  <si>
+    <t>value 10</t>
   </si>
 </sst>
 </file>
@@ -404,14 +410,14 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1">
-        <v>999</v>
+      <c r="A1" t="s">
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -485,8 +491,8 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>100</v>
+      <c r="B10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>